<commit_message>
Update report using partial correlation
</commit_message>
<xml_diff>
--- a/Q7/Correlation.xlsx
+++ b/Q7/Correlation.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hpbui/Code/BigData/P2-hiep_alper_team_project2/Q7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1EBAC69-7901-394E-8206-DB13EEE570DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A39935B-0B0D-2749-BD3A-BDC4B92EA131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15660" xr2:uid="{DA387473-1A76-6B48-A172-ED567EBA6E0E}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15660" activeTab="1" xr2:uid="{DA387473-1A76-6B48-A172-ED567EBA6E0E}"/>
   </bookViews>
   <sheets>
     <sheet name="All feature" sheetId="1" r:id="rId1"/>
+    <sheet name="Partial" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="113">
   <si>
     <t>utc_date,utc_time</t>
   </si>
@@ -377,7 +378,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -410,7 +411,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,7 +421,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.000000"/>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -455,6 +456,29 @@
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D351BA85-7421-FB43-8941-E099AE83174E}" name="Table2" displayName="Table2" ref="A1:C43" totalsRowShown="0">
+  <autoFilter ref="A1:C43" xr:uid="{C019D910-3F82-594D-AFC3-ECD3C442EA2D}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="0"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C42">
+    <sortCondition descending="1" ref="B1:B43"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{B4FE7450-3863-194A-9CB0-174F635EBC21}" name="Type"/>
+    <tableColumn id="2" xr3:uid="{68631DE6-C155-8046-A896-FC409C5A8EA3}" name="Correlation"/>
+    <tableColumn id="3" xr3:uid="{561D2334-2331-C544-A20F-3C07767C4F7E}" name="Helper Column">
+      <calculatedColumnFormula>MOD(ROW(),2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -757,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{061D802D-4FB7-0749-BBCE-193A4E125DD2}">
   <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2104,4 +2128,542 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B8CA49-0EA0-0E45-B279-F810E1AC3D14}">
+  <dimension ref="A1:C43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2">
+        <v>0.96922612117608598</v>
+      </c>
+      <c r="C2">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3">
+        <v>3.1841396538457398E-2</v>
+      </c>
+      <c r="C3">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4">
+        <v>0.57936426714765998</v>
+      </c>
+      <c r="C4">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5">
+        <v>0.42730046286332402</v>
+      </c>
+      <c r="C5">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6">
+        <v>0.431872237039161</v>
+      </c>
+      <c r="C6">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7">
+        <v>0.96922612117608598</v>
+      </c>
+      <c r="C7">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8">
+        <v>0.42730046286332402</v>
+      </c>
+      <c r="C8">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9">
+        <v>0.354089708501308</v>
+      </c>
+      <c r="C9">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10">
+        <v>0.37212995125054599</v>
+      </c>
+      <c r="C10">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11">
+        <v>0.36056980432860902</v>
+      </c>
+      <c r="C11">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12">
+        <v>0.36056980432860902</v>
+      </c>
+      <c r="C12">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13">
+        <v>7.3962553953952404E-2</v>
+      </c>
+      <c r="C13">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14">
+        <v>0.354089708501308</v>
+      </c>
+      <c r="C14">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15">
+        <v>3.2673889903086999E-2</v>
+      </c>
+      <c r="C15">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B16">
+        <v>0.34818599803428602</v>
+      </c>
+      <c r="C16">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17">
+        <v>2.5126990292173301E-2</v>
+      </c>
+      <c r="C17">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18">
+        <v>0.29310840897444301</v>
+      </c>
+      <c r="C18">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19">
+        <v>5.3260043795434801E-2</v>
+      </c>
+      <c r="C19">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20">
+        <v>0.28244620617513</v>
+      </c>
+      <c r="C20">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21">
+        <v>0.11182291384506</v>
+      </c>
+      <c r="C21">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22">
+        <v>0.19297770232780601</v>
+      </c>
+      <c r="C22">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B23">
+        <v>2.1674276789151901E-3</v>
+      </c>
+      <c r="C23">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24">
+        <v>0.11182291384506</v>
+      </c>
+      <c r="C24">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25">
+        <v>0.57936426714765998</v>
+      </c>
+      <c r="C25">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26">
+        <v>0.110007263519114</v>
+      </c>
+      <c r="C26">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27">
+        <v>0.431872237039161</v>
+      </c>
+      <c r="C27">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28">
+        <v>7.3962553953952404E-2</v>
+      </c>
+      <c r="C28">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29">
+        <v>0.28244620617513</v>
+      </c>
+      <c r="C29">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>106</v>
+      </c>
+      <c r="B30">
+        <v>6.5867831101036195E-2</v>
+      </c>
+      <c r="C30">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B31">
+        <v>0.110007263519114</v>
+      </c>
+      <c r="C31">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>84</v>
+      </c>
+      <c r="B32">
+        <v>5.3260043795434801E-2</v>
+      </c>
+      <c r="C32">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33">
+        <v>0.37212995125054599</v>
+      </c>
+      <c r="C33">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34">
+        <v>3.8596059729745197E-2</v>
+      </c>
+      <c r="C34">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B35">
+        <v>0.34818599803428602</v>
+      </c>
+      <c r="C35">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36">
+        <v>3.2673889903086999E-2</v>
+      </c>
+      <c r="C36">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37">
+        <v>3.8596059729745197E-2</v>
+      </c>
+      <c r="C37">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38">
+        <v>3.1841396538457398E-2</v>
+      </c>
+      <c r="C38">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>105</v>
+      </c>
+      <c r="B39">
+        <v>0.29310840897444301</v>
+      </c>
+      <c r="C39">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40">
+        <v>2.5126990292173301E-2</v>
+      </c>
+      <c r="C40">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>107</v>
+      </c>
+      <c r="B41">
+        <v>6.5867831101036195E-2</v>
+      </c>
+      <c r="C41">
+        <f>MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>88</v>
+      </c>
+      <c r="B42">
+        <v>2.1674276789151901E-3</v>
+      </c>
+      <c r="C42">
+        <f>MOD(ROW(),2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>109</v>
+      </c>
+      <c r="B43">
+        <v>0.19297770232780601</v>
+      </c>
+      <c r="C43">
+        <f t="shared" ref="C3:C43" si="0">MOD(ROW(),2)</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update report for correlation table
</commit_message>
<xml_diff>
--- a/Q7/Correlation.xlsx
+++ b/Q7/Correlation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hpbui/Code/BigData/P2-hiep_alper_team_project2/Q7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A39935B-0B0D-2749-BD3A-BDC4B92EA131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C059F66D-1FDA-A942-82E9-94E907C67714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15660" activeTab="1" xr2:uid="{DA387473-1A76-6B48-A172-ED567EBA6E0E}"/>
   </bookViews>
@@ -2135,7 +2135,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2164,7 +2164,7 @@
         <v>0.96922612117608598</v>
       </c>
       <c r="C2">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" ref="C2:C42" si="0">MOD(ROW(),2)</f>
         <v>0</v>
       </c>
     </row>
@@ -2176,7 +2176,7 @@
         <v>3.1841396538457398E-2</v>
       </c>
       <c r="C3">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2188,7 +2188,7 @@
         <v>0.57936426714765998</v>
       </c>
       <c r="C4">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2200,7 +2200,7 @@
         <v>0.42730046286332402</v>
       </c>
       <c r="C5">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2212,7 +2212,7 @@
         <v>0.431872237039161</v>
       </c>
       <c r="C6">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2224,7 +2224,7 @@
         <v>0.96922612117608598</v>
       </c>
       <c r="C7">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2236,7 +2236,7 @@
         <v>0.42730046286332402</v>
       </c>
       <c r="C8">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2248,7 +2248,7 @@
         <v>0.354089708501308</v>
       </c>
       <c r="C9">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2260,7 +2260,7 @@
         <v>0.37212995125054599</v>
       </c>
       <c r="C10">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2272,7 +2272,7 @@
         <v>0.36056980432860902</v>
       </c>
       <c r="C11">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2284,7 +2284,7 @@
         <v>0.36056980432860902</v>
       </c>
       <c r="C12">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2296,7 +2296,7 @@
         <v>7.3962553953952404E-2</v>
       </c>
       <c r="C13">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2308,7 +2308,7 @@
         <v>0.354089708501308</v>
       </c>
       <c r="C14">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2320,7 +2320,7 @@
         <v>3.2673889903086999E-2</v>
       </c>
       <c r="C15">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2332,7 +2332,7 @@
         <v>0.34818599803428602</v>
       </c>
       <c r="C16">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2344,7 +2344,7 @@
         <v>2.5126990292173301E-2</v>
       </c>
       <c r="C17">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2356,7 +2356,7 @@
         <v>0.29310840897444301</v>
       </c>
       <c r="C18">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2368,7 +2368,7 @@
         <v>5.3260043795434801E-2</v>
       </c>
       <c r="C19">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2380,7 +2380,7 @@
         <v>0.28244620617513</v>
       </c>
       <c r="C20">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2392,7 +2392,7 @@
         <v>0.11182291384506</v>
       </c>
       <c r="C21">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2404,7 +2404,7 @@
         <v>0.19297770232780601</v>
       </c>
       <c r="C22">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2416,7 +2416,7 @@
         <v>2.1674276789151901E-3</v>
       </c>
       <c r="C23">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2428,7 +2428,7 @@
         <v>0.11182291384506</v>
       </c>
       <c r="C24">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2440,7 +2440,7 @@
         <v>0.57936426714765998</v>
       </c>
       <c r="C25">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2452,7 +2452,7 @@
         <v>0.110007263519114</v>
       </c>
       <c r="C26">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2464,7 +2464,7 @@
         <v>0.431872237039161</v>
       </c>
       <c r="C27">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2476,7 +2476,7 @@
         <v>7.3962553953952404E-2</v>
       </c>
       <c r="C28">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2488,7 +2488,7 @@
         <v>0.28244620617513</v>
       </c>
       <c r="C29">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2500,7 +2500,7 @@
         <v>6.5867831101036195E-2</v>
       </c>
       <c r="C30">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2512,7 +2512,7 @@
         <v>0.110007263519114</v>
       </c>
       <c r="C31">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2524,7 +2524,7 @@
         <v>5.3260043795434801E-2</v>
       </c>
       <c r="C32">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2536,7 +2536,7 @@
         <v>0.37212995125054599</v>
       </c>
       <c r="C33">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2548,7 +2548,7 @@
         <v>3.8596059729745197E-2</v>
       </c>
       <c r="C34">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2560,7 +2560,7 @@
         <v>0.34818599803428602</v>
       </c>
       <c r="C35">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2572,7 +2572,7 @@
         <v>3.2673889903086999E-2</v>
       </c>
       <c r="C36">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2584,7 +2584,7 @@
         <v>3.8596059729745197E-2</v>
       </c>
       <c r="C37">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2596,7 +2596,7 @@
         <v>3.1841396538457398E-2</v>
       </c>
       <c r="C38">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2608,7 +2608,7 @@
         <v>0.29310840897444301</v>
       </c>
       <c r="C39">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2620,7 +2620,7 @@
         <v>2.5126990292173301E-2</v>
       </c>
       <c r="C40">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2632,7 +2632,7 @@
         <v>6.5867831101036195E-2</v>
       </c>
       <c r="C41">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -2644,7 +2644,7 @@
         <v>2.1674276789151901E-3</v>
       </c>
       <c r="C42">
-        <f>MOD(ROW(),2)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2656,7 +2656,7 @@
         <v>0.19297770232780601</v>
       </c>
       <c r="C43">
-        <f t="shared" ref="C3:C43" si="0">MOD(ROW(),2)</f>
+        <f t="shared" ref="C43" si="1">MOD(ROW(),2)</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>